<commit_message>
Traffic Accidents - data updates and rf model
</commit_message>
<xml_diff>
--- a/TrafficAccidents/data/BankHolidaysScotland.xlsx
+++ b/TrafficAccidents/data/BankHolidaysScotland.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0AA68BA5-8079-424B-99FC-01A6F7EA5AE7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A5F763A5-862D-4033-99EA-3CB8143C4957}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -341,10 +341,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A112"/>
+  <dimension ref="A1:A139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
-      <selection activeCell="A112" sqref="A112"/>
+    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
+      <selection activeCell="A139" sqref="A139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -912,6 +912,141 @@
         <v>38713</v>
       </c>
     </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A113" s="1">
+        <v>42738</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A114" s="1">
+        <v>42737</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A115" s="1">
+        <v>42839</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A116" s="1">
+        <v>42856</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A117" s="1">
+        <v>42884</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A118" s="1">
+        <v>42954</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A119" s="1">
+        <v>43069</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A120" s="1">
+        <v>43094</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A121" s="1">
+        <v>43095</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A122" s="1">
+        <v>43101</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A123" s="1">
+        <v>43102</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A124" s="1">
+        <v>43189</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A125" s="1">
+        <v>43227</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A126" s="1">
+        <v>43248</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A127" s="1">
+        <v>43318</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A128" s="1">
+        <v>43434</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A129" s="1">
+        <v>43459</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A130" s="1">
+        <v>43460</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A131" s="1">
+        <v>43466</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A132" s="1">
+        <v>43467</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A133" s="1">
+        <v>43574</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A134" s="1">
+        <v>43591</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A135" s="1">
+        <v>43612</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A136" s="1">
+        <v>43682</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A137" s="1">
+        <v>43801</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A138" s="1">
+        <v>43824</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A139" s="1">
+        <v>43825</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>